<commit_message>
Updated data with mRMR runs
</commit_message>
<xml_diff>
--- a/Code/R/Magnan/AntigenPro_IT.xlsx
+++ b/Code/R/Magnan/AntigenPro_IT.xlsx
@@ -4,13 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7995" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7995" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Score" sheetId="2" r:id="rId1"/>
     <sheet name="Enrichment" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
-    <sheet name="Performance" sheetId="5" r:id="rId4"/>
+    <sheet name="Performance" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -6890,23 +6889,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="59692160"/>
-        <c:axId val="59694080"/>
+        <c:axId val="70802048"/>
+        <c:axId val="70828416"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="59692160"/>
+        <c:axId val="70802048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59694080"/>
+        <c:crossAx val="70828416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="59694080"/>
+        <c:axId val="70828416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6914,20 +6913,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59692160"/>
+        <c:crossAx val="70802048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -24196,18 +24194,6 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">

</xml_diff>